<commit_message>
Ignore degenerate neighbors in GPU k-NN kernel
</commit_message>
<xml_diff>
--- a/test/knn_test_verification.xlsx
+++ b/test/knn_test_verification.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keichi/Projects/research/cuEDM/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D757E7D4-1BE7-5140-A0C4-AED90CC27406}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD37D691-5BCB-6F49-929E-7B9571B4B82C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40960" yWindow="540" windowWidth="25200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31820" yWindow="1120" windowWidth="25200" windowHeight="28340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>E = 2</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>Top5</t>
   </si>
 </sst>
 </file>
@@ -898,7 +901,7 @@
   <dimension ref="A1:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24:N32"/>
+      <selection activeCell="N54" sqref="N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1386,6 +1389,9 @@
       <c r="N13" t="s">
         <v>7</v>
       </c>
+      <c r="O13" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
@@ -1429,16 +1435,20 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <f>SMALL(A14:I14, 2)</f>
+        <f>SMALL($A14:$I14, 2)</f>
         <v>0.16593352820162913</v>
       </c>
       <c r="M14">
-        <f>SMALL(A14:I14, 3)</f>
+        <f>SMALL($A14:$I14, 3)</f>
         <v>0.32794322883922516</v>
       </c>
       <c r="N14">
-        <f>SMALL(A14:I14, 4)</f>
+        <f>SMALL($A14:$I14, 4)</f>
         <v>0.37845509134781247</v>
+      </c>
+      <c r="O14">
+        <f>SMALL($A14:$I14, 5)</f>
+        <v>0.41934204867047936</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
@@ -1483,16 +1493,20 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:L22" si="15">SMALL(A15:I15, 2)</f>
+        <f t="shared" ref="L15:L22" si="15">SMALL($A15:$I15, 2)</f>
         <v>0.27588630667263342</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M22" si="16">SMALL(A15:I15, 3)</f>
+        <f t="shared" ref="M15:M22" si="16">SMALL($A15:$I15, 3)</f>
         <v>0.38432734795556989</v>
       </c>
       <c r="N15">
-        <f t="shared" ref="N15:N22" si="17">SMALL(A15:I15, 4)</f>
+        <f t="shared" ref="N15:N22" si="17">SMALL($A15:$I15, 4)</f>
         <v>0.41934204867047936</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ref="O15:O22" si="18">SMALL($A15:$I15, 5)</f>
+        <v>0.56861588715014488</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
@@ -1548,8 +1562,12 @@
         <f t="shared" si="17"/>
         <v>0.49246986770470541</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O16">
+        <f t="shared" si="18"/>
+        <v>0.50614990517288549</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17">
         <f>SQRT(SUMXMY2(C3:D3,C6:D6))</f>
         <v>0.67515012475130198</v>
@@ -1602,8 +1620,12 @@
         <f t="shared" si="17"/>
         <v>0.59605636702837694</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O17">
+        <f t="shared" si="18"/>
+        <v>0.67515012475130198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>SQRT(SUMXMY2(C3:D3,C7:D7))</f>
         <v>0.45397053115583175</v>
@@ -1656,8 +1678,12 @@
         <f t="shared" si="17"/>
         <v>0.49246986770470541</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O18">
+        <f t="shared" si="18"/>
+        <v>0.5924232482109214</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19">
         <f>SQRT(SUMXMY2(C3:D3,C8:D8))</f>
         <v>0.16593352820162913</v>
@@ -1710,8 +1736,12 @@
         <f t="shared" si="17"/>
         <v>0.4025028204115445</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O19">
+        <f t="shared" si="18"/>
+        <v>0.493821911915312</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20">
         <f>SQRT(SUMXMY2(C3:D3,C9:D9))</f>
         <v>0.37845509134781247</v>
@@ -1764,8 +1794,12 @@
         <f t="shared" si="17"/>
         <v>0.37845509134781247</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O20">
+        <f t="shared" si="18"/>
+        <v>0.53061013321840234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21">
         <f>SQRT(SUMXMY2(C3:D3,C10:D10))</f>
         <v>0.43802207706394858</v>
@@ -1818,8 +1852,12 @@
         <f t="shared" si="17"/>
         <v>0.51157953137035073</v>
       </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O21">
+        <f t="shared" si="18"/>
+        <v>0.53087345360504423</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22">
         <f>SQRT(SUMXMY2(C3:D3,C11:D11))</f>
         <v>0.32794322883922516</v>
@@ -1872,8 +1910,12 @@
         <f t="shared" si="17"/>
         <v>0.43765923506981824</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O22">
+        <f t="shared" si="18"/>
+        <v>0.45513617287030267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>1</v>
       </c>
@@ -1889,8 +1931,11 @@
       <c r="N24" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25">
         <f>SQRT(SUMXMY2(F3:H3,F3:H3))</f>
         <v>0</v>
@@ -1928,19 +1973,23 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <f>SMALL(A25:H25, 2)</f>
+        <f>SMALL($A25:$I25, 2)</f>
         <v>0.51534002939654799</v>
       </c>
       <c r="M25">
-        <f>SMALL(A25:H25, 3)</f>
+        <f>SMALL($A25:$I25, 3)</f>
         <v>0.51951597653577219</v>
       </c>
       <c r="N25">
-        <f>SMALL(A25:H25, 4)</f>
+        <f>SMALL($A25:$I25, 4)</f>
         <v>0.575806941173715</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O25">
+        <f>SMALL($A25:$I25, 5)</f>
+        <v>0.73982317664384623</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26">
         <f>SQRT(SUMXMY2(F3:H3,F4:H4))</f>
         <v>0.89029510101964504</v>
@@ -1974,23 +2023,27 @@
         <v>0.57144050943619307</v>
       </c>
       <c r="K26">
-        <f t="shared" ref="K26:K32" si="18">SMALL(A26:H26, 1)</f>
+        <f t="shared" ref="K26:K32" si="19">SMALL(A26:H26, 1)</f>
         <v>0</v>
       </c>
       <c r="L26">
-        <f t="shared" ref="L26:L32" si="19">SMALL(A26:H26, 2)</f>
+        <f t="shared" ref="L26:L32" si="20">SMALL($A26:$I26, 2)</f>
         <v>0.27592287700068935</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26:M32" si="20">SMALL(A26:H26, 3)</f>
+        <f t="shared" ref="M26:M32" si="21">SMALL($A26:$I26, 3)</f>
         <v>0.57144050943619307</v>
       </c>
       <c r="N26">
-        <f t="shared" ref="N26:N32" si="21">SMALL(A26:H26, 4)</f>
+        <f t="shared" ref="N26:N32" si="22">SMALL($A26:$I26, 4)</f>
         <v>0.6171275893943956</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O26">
+        <f t="shared" ref="O26:O32" si="23">SMALL($A26:$I26, 5)</f>
+        <v>0.79735056332904242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27">
         <f>SQRT(SUMXMY2(F3:H3,F5:H5))</f>
         <v>0.51534002939654799</v>
@@ -2024,23 +2077,27 @@
         <v>1.18939317481188</v>
       </c>
       <c r="K27">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.51534002939654799</v>
       </c>
       <c r="M27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.58790665114502327</v>
       </c>
       <c r="N27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.6038797993532995</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O27">
+        <f t="shared" si="23"/>
+        <v>1.0704099756957917</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28">
         <f>SQRT(SUMXMY2(F3:H3,F6:H6))</f>
         <v>0.73982317664384623</v>
@@ -2074,23 +2131,27 @@
         <v>0.68072444978682423</v>
       </c>
       <c r="K28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.6171275893943956</v>
       </c>
       <c r="M28">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.68072444978682423</v>
       </c>
       <c r="N28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.73982317664384623</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O28">
+        <f t="shared" si="23"/>
+        <v>0.76426713669106239</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29">
         <f>SQRT(SUMXMY2(F3:H3,F7:H7))</f>
         <v>0.51951597653577219</v>
@@ -2124,23 +2185,27 @@
         <v>1.0071266800035708</v>
       </c>
       <c r="K29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.51951597653577219</v>
       </c>
       <c r="M29">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.6038797993532995</v>
       </c>
       <c r="N29">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.61956263475697027</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O29">
+        <f t="shared" si="23"/>
+        <v>0.6641272970588763</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30">
         <f>SQRT(SUMXMY2(F3:H3,F8:H8))</f>
         <v>0.79829556947026037</v>
@@ -2174,23 +2239,27 @@
         <v>0.51424137077372234</v>
       </c>
       <c r="K30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.27592287700068935</v>
       </c>
       <c r="M30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.51424137077372234</v>
       </c>
       <c r="N30">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.63394262002154489</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O30">
+        <f t="shared" si="23"/>
+        <v>0.6641272970588763</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>SQRT(SUMXMY2(F3:H3,F9:H9))</f>
         <v>0.575806941173715</v>
@@ -2224,23 +2293,27 @@
         <v>0.69728436244799497</v>
       </c>
       <c r="K31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L31">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.575806941173715</v>
       </c>
       <c r="M31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.58790665114502327</v>
       </c>
       <c r="N31">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.61956263475697027</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O31">
+        <f t="shared" si="23"/>
+        <v>0.63394262002154489</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32">
         <f>SQRT(SUMXMY2(F3:H3,F10:H10))</f>
         <v>0.85013431888901514</v>
@@ -2274,23 +2347,27 @@
         <v>0</v>
       </c>
       <c r="K32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="L32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.51424137077372234</v>
       </c>
       <c r="M32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.57144050943619307</v>
       </c>
       <c r="N32">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0.68072444978682423</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O32">
+        <f t="shared" si="23"/>
+        <v>0.69728436244799497</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -2306,8 +2383,11 @@
       <c r="N34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35">
         <f>SQRT(SUMXMY2(J3:M3,J3:M3))</f>
         <v>0</v>
@@ -2341,19 +2421,23 @@
         <v>0</v>
       </c>
       <c r="L35">
-        <f>SMALL(A35:G35, 2)</f>
+        <f>SMALL($A35:$I35, 2)</f>
         <v>0.51953539794588421</v>
       </c>
       <c r="M35">
-        <f>SMALL(A35:G35, 3)</f>
+        <f>SMALL($A35:$I35, 3)</f>
         <v>0.57859645886315236</v>
       </c>
       <c r="N35">
-        <f>SMALL(A35:G35, 4)</f>
+        <f>SMALL($A35:$I35, 4)</f>
         <v>0.70619706676225369</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35">
+        <f>SMALL($A35:$I35, 5)</f>
+        <v>0.87220913204235118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36">
         <f>SQRT(SUMXMY2(J3:M3,J4:M4))</f>
         <v>1.2533856805204069</v>
@@ -2383,23 +2467,27 @@
         <v>1.2002185108487871</v>
       </c>
       <c r="K36">
-        <f t="shared" ref="K36:K41" si="22">SMALL(A36:G36, 1)</f>
+        <f t="shared" ref="K36:K41" si="24">SMALL(A36:G36, 1)</f>
         <v>0</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L36:L41" si="23">SMALL(A36:G36, 2)</f>
+        <f t="shared" ref="L36:L41" si="25">SMALL($A36:$I36, 2)</f>
         <v>0.59828076849587386</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M36:M41" si="24">SMALL(A36:G36, 3)</f>
+        <f t="shared" ref="M36:M41" si="26">SMALL($A36:$I36, 3)</f>
         <v>0.70921837473491123</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N36:N41" si="25">SMALL(A36:G36, 4)</f>
+        <f t="shared" ref="N36:N41" si="27">SMALL($A36:$I36, 4)</f>
         <v>1.185838095917171</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O36">
+        <f t="shared" ref="O36:O41" si="28">SMALL($A36:$I36, 5)</f>
+        <v>1.2002185108487871</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37">
         <f>SQRT(SUMXMY2(J3:M3,J5:M5))</f>
         <v>0.70619706676225369</v>
@@ -2429,23 +2517,27 @@
         <v>0.72608083796198852</v>
       </c>
       <c r="K37">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L37">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.70619706676225369</v>
       </c>
       <c r="M37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.72608083796198852</v>
       </c>
       <c r="N37">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.77038423894694852</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O37">
+        <f t="shared" si="28"/>
+        <v>1.0784519367402134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38">
         <f>SQRT(SUMXMY2(J3:M3,J6:M6))</f>
         <v>0.91168039253536859</v>
@@ -2475,23 +2567,27 @@
         <v>1.139353744457386</v>
       </c>
       <c r="K38">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L38">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.70921837473491123</v>
       </c>
       <c r="M38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.7854914446333422</v>
       </c>
       <c r="N38">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.91168039253536859</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O38">
+        <f t="shared" si="28"/>
+        <v>1.1042714176925674</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39">
         <f>SQRT(SUMXMY2(J3:M3,J7:M7))</f>
         <v>0.51953539794588421</v>
@@ -2521,23 +2617,27 @@
         <v>0.62176235724360818</v>
       </c>
       <c r="K39">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L39">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.51953539794588421</v>
       </c>
       <c r="M39">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.62176235724360818</v>
       </c>
       <c r="N39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.74926710771557226</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O39">
+        <f t="shared" si="28"/>
+        <v>0.77038423894694852</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40">
         <f>SQRT(SUMXMY2(J3:M3,J8:M8))</f>
         <v>0.87220913204235118</v>
@@ -2567,23 +2667,27 @@
         <v>0.69906798619953747</v>
       </c>
       <c r="K40">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L40">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.59828076849587386</v>
       </c>
       <c r="M40">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.69906798619953747</v>
       </c>
       <c r="N40">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.74926710771557226</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O40">
+        <f t="shared" si="28"/>
+        <v>0.7854914446333422</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41">
         <f>SQRT(SUMXMY2(J3:M3,J9:M9))</f>
         <v>0.57859645886315236</v>
@@ -2613,23 +2717,27 @@
         <v>0</v>
       </c>
       <c r="K41">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L41">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.57859645886315236</v>
       </c>
       <c r="M41">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>0.62176235724360818</v>
       </c>
       <c r="N41">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>0.69906798619953747</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O41">
+        <f t="shared" si="28"/>
+        <v>0.72608083796198852</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>3</v>
       </c>
@@ -2645,8 +2753,11 @@
       <c r="N43" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O43" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44">
         <f>SQRT(SUMXMY2(O3:S3,O3:S3))</f>
         <v>0</v>
@@ -2676,19 +2787,23 @@
         <v>0</v>
       </c>
       <c r="L44">
-        <f>SMALL(A44:F44, 2)</f>
+        <f>SMALL($A44:$I44, 2)</f>
         <v>0.74278090552898846</v>
       </c>
       <c r="M44">
-        <f>SMALL(A44:F44, 3)</f>
+        <f>SMALL($A44:$I44, 3)</f>
         <v>0.78794577134058041</v>
       </c>
       <c r="N44">
-        <f>SMALL(A44:F44, 4)</f>
+        <f>SMALL($A44:$I44, 4)</f>
         <v>1.2009121783338381</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O44">
+        <f>SMALL($A44:$I44, 5)</f>
+        <v>1.2655454187901611</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45">
         <f>SQRT(SUMXMY2(O3:S3,O4:S4))</f>
         <v>1.3154822755773952</v>
@@ -2714,23 +2829,27 @@
         <v>0.73450597733921863</v>
       </c>
       <c r="K45">
-        <f t="shared" ref="K45:K49" si="26">SMALL(A45:F45, 1)</f>
+        <f t="shared" ref="K45:K49" si="29">SMALL(A45:F45, 1)</f>
         <v>0</v>
       </c>
       <c r="L45">
-        <f t="shared" ref="L45:L49" si="27">SMALL(A45:F45, 2)</f>
+        <f t="shared" ref="L45:L49" si="30">SMALL($A45:$I45, 2)</f>
         <v>0.73450597733921863</v>
       </c>
       <c r="M45">
-        <f t="shared" ref="M45:M49" si="28">SMALL(A45:F45, 3)</f>
+        <f t="shared" ref="M45:M49" si="31">SMALL($A45:$I45, 3)</f>
         <v>0.8554599737056765</v>
       </c>
       <c r="N45">
-        <f t="shared" ref="N45:N49" si="29">SMALL(A45:F45, 4)</f>
+        <f t="shared" ref="N45:N49" si="32">SMALL($A45:$I45, 4)</f>
         <v>1.1931022812475522</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O45">
+        <f t="shared" ref="O45:O49" si="33">SMALL($A45:$I45, 5)</f>
+        <v>1.314559804055158</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46">
         <f>SQRT(SUMXMY2(O3:S3,O5:S5))</f>
         <v>0.78794577134058041</v>
@@ -2756,23 +2875,27 @@
         <v>1.1788289090265642</v>
       </c>
       <c r="K46">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L46">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0.78794577134058041</v>
       </c>
       <c r="M46">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.79144452047132718</v>
       </c>
       <c r="N46">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>1.1788289090265642</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O46">
+        <f t="shared" si="33"/>
+        <v>1.314559804055158</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47">
         <f>SQRT(SUMXMY2(O3:S3,O6:S6))</f>
         <v>1.2655454187901611</v>
@@ -2798,23 +2921,27 @@
         <v>0.78722765455127675</v>
       </c>
       <c r="K47">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L47">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0.78722765455127675</v>
       </c>
       <c r="M47">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.8554599737056765</v>
       </c>
       <c r="N47">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>1.1574763478959225</v>
       </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O47">
+        <f t="shared" si="33"/>
+        <v>1.2655454187901611</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48">
         <f>SQRT(SUMXMY2(O3:S3,O7:S7))</f>
         <v>0.74278090552898846</v>
@@ -2840,23 +2967,27 @@
         <v>0.80511738433209534</v>
       </c>
       <c r="K48">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L48">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0.74278090552898846</v>
       </c>
       <c r="M48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.79144452047132718</v>
       </c>
       <c r="N48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.80511738433209534</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O48">
+        <f t="shared" si="33"/>
+        <v>1.1574763478959225</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49">
         <f>SQRT(SUMXMY2(O3:S3,O8:S8))</f>
         <v>1.2009121783338381</v>
@@ -2882,20 +3013,24 @@
         <v>0</v>
       </c>
       <c r="K49">
-        <f t="shared" si="26"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="L49">
-        <f t="shared" si="27"/>
+        <f t="shared" si="30"/>
         <v>0.73450597733921863</v>
       </c>
       <c r="M49">
-        <f t="shared" si="28"/>
+        <f t="shared" si="31"/>
         <v>0.78722765455127675</v>
       </c>
       <c r="N49">
-        <f t="shared" si="29"/>
+        <f t="shared" si="32"/>
         <v>0.80511738433209534</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="33"/>
+        <v>1.1788289090265642</v>
       </c>
     </row>
   </sheetData>

</xml_diff>